<commit_message>
new test case is added for Login functionality
</commit_message>
<xml_diff>
--- a/Testc.xlsx
+++ b/Testc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Haripemireddy\QATraining\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E1242A8-6DCD-4DD9-B2F3-A89F84F444A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A9DA766-8A8D-482B-A9F9-58C0B966C349}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="247">
   <si>
     <t>S.No</t>
   </si>
@@ -816,6 +816,38 @@
   <si>
     <t>Password input box should display hint
 word"Password"</t>
+  </si>
+  <si>
+    <t>To verify the remember me check box is deselect</t>
+  </si>
+  <si>
+    <t>2.Valid email and password</t>
+  </si>
+  <si>
+    <t>1.new page open with "welcome 
+to Auto tools" message</t>
+  </si>
+  <si>
+    <t>1.Click on Sign in</t>
+  </si>
+  <si>
+    <t>2.Close the browser</t>
+  </si>
+  <si>
+    <t>2.Browser is closed</t>
+  </si>
+  <si>
+    <t>3.open the browser</t>
+  </si>
+  <si>
+    <t>4.enter the Url</t>
+  </si>
+  <si>
+    <t>3.Login page is opened</t>
+  </si>
+  <si>
+    <t>Browser should not remember Email 
+and password</t>
   </si>
 </sst>
 </file>
@@ -969,7 +1001,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1118,6 +1150,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1133,88 +1169,88 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1560,10 +1596,10 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="57" t="s">
+      <c r="E1" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="57"/>
+      <c r="F1" s="59"/>
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1598,13 +1634,13 @@
       <c r="F4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="55" t="s">
+      <c r="G4" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="55" t="s">
+      <c r="H4" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="56" t="s">
+      <c r="I4" s="58" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1615,9 +1651,9 @@
       <c r="F5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="55"/>
-      <c r="H5" s="55"/>
-      <c r="I5" s="56"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="58"/>
     </row>
     <row r="6" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="E6" s="4" t="s">
@@ -1626,9 +1662,9 @@
       <c r="F6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="56"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="58"/>
     </row>
     <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
@@ -1646,13 +1682,13 @@
       <c r="F9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="55" t="s">
+      <c r="G9" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="56" t="s">
+      <c r="H9" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="56" t="s">
+      <c r="I9" s="58" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1663,9 +1699,9 @@
       <c r="F10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="55"/>
-      <c r="H10" s="56"/>
-      <c r="I10" s="56"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="58"/>
+      <c r="I10" s="58"/>
     </row>
     <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="E11" s="4" t="s">
@@ -1674,9 +1710,9 @@
       <c r="F11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="55"/>
-      <c r="H11" s="56"/>
-      <c r="I11" s="56"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="58"/>
+      <c r="I11" s="58"/>
     </row>
     <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="E12" s="4" t="s">
@@ -1685,9 +1721,9 @@
       <c r="F12" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="55"/>
-      <c r="H12" s="56"/>
-      <c r="I12" s="56"/>
+      <c r="G12" s="57"/>
+      <c r="H12" s="58"/>
+      <c r="I12" s="58"/>
     </row>
     <row r="13" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="E13" s="3" t="s">
@@ -1696,9 +1732,9 @@
       <c r="F13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G13" s="55"/>
-      <c r="H13" s="56"/>
-      <c r="I13" s="56"/>
+      <c r="G13" s="57"/>
+      <c r="H13" s="58"/>
+      <c r="I13" s="58"/>
     </row>
     <row r="16" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
@@ -1716,13 +1752,13 @@
       <c r="F16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="55" t="s">
+      <c r="G16" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="H16" s="56" t="s">
+      <c r="H16" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="I16" s="56" t="s">
+      <c r="I16" s="58" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1733,9 +1769,9 @@
       <c r="F17" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G17" s="55"/>
-      <c r="H17" s="56"/>
-      <c r="I17" s="56"/>
+      <c r="G17" s="57"/>
+      <c r="H17" s="58"/>
+      <c r="I17" s="58"/>
     </row>
     <row r="18" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="E18" s="4" t="s">
@@ -1744,9 +1780,9 @@
       <c r="F18" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G18" s="55"/>
-      <c r="H18" s="56"/>
-      <c r="I18" s="56"/>
+      <c r="G18" s="57"/>
+      <c r="H18" s="58"/>
+      <c r="I18" s="58"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="E19" s="4" t="s">
@@ -1755,9 +1791,9 @@
       <c r="F19" t="s">
         <v>26</v>
       </c>
-      <c r="G19" s="55"/>
-      <c r="H19" s="56"/>
-      <c r="I19" s="56"/>
+      <c r="G19" s="57"/>
+      <c r="H19" s="58"/>
+      <c r="I19" s="58"/>
     </row>
     <row r="22" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
@@ -1778,13 +1814,13 @@
       <c r="F22" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G22" s="55" t="s">
+      <c r="G22" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="H22" s="56" t="s">
+      <c r="H22" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="I22" s="56" t="s">
+      <c r="I22" s="58" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1795,9 +1831,9 @@
       <c r="F23" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G23" s="55"/>
-      <c r="H23" s="56"/>
-      <c r="I23" s="56"/>
+      <c r="G23" s="57"/>
+      <c r="H23" s="58"/>
+      <c r="I23" s="58"/>
     </row>
     <row r="24" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="E24" s="4" t="s">
@@ -1806,9 +1842,9 @@
       <c r="F24" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G24" s="55"/>
-      <c r="H24" s="56"/>
-      <c r="I24" s="56"/>
+      <c r="G24" s="57"/>
+      <c r="H24" s="58"/>
+      <c r="I24" s="58"/>
     </row>
     <row r="25" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="E25" s="4" t="s">
@@ -1817,9 +1853,9 @@
       <c r="F25" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G25" s="55"/>
-      <c r="H25" s="56"/>
-      <c r="I25" s="56"/>
+      <c r="G25" s="57"/>
+      <c r="H25" s="58"/>
+      <c r="I25" s="58"/>
     </row>
     <row r="28" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
@@ -1837,13 +1873,13 @@
       <c r="F28" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G28" s="55" t="s">
+      <c r="G28" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="H28" s="55" t="s">
+      <c r="H28" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="I28" s="56" t="s">
+      <c r="I28" s="58" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1854,9 +1890,9 @@
       <c r="F29" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G29" s="55"/>
-      <c r="H29" s="55"/>
-      <c r="I29" s="56"/>
+      <c r="G29" s="57"/>
+      <c r="H29" s="57"/>
+      <c r="I29" s="58"/>
     </row>
     <row r="30" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="E30" s="4" t="s">
@@ -1865,9 +1901,9 @@
       <c r="F30" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G30" s="55"/>
-      <c r="H30" s="55"/>
-      <c r="I30" s="56"/>
+      <c r="G30" s="57"/>
+      <c r="H30" s="57"/>
+      <c r="I30" s="58"/>
     </row>
     <row r="31" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="E31" s="4" t="s">
@@ -1876,9 +1912,9 @@
       <c r="F31" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G31" s="55"/>
-      <c r="H31" s="55"/>
-      <c r="I31" s="56"/>
+      <c r="G31" s="57"/>
+      <c r="H31" s="57"/>
+      <c r="I31" s="58"/>
     </row>
     <row r="34" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A34">
@@ -1896,13 +1932,13 @@
       <c r="F34" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G34" s="55" t="s">
+      <c r="G34" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="H34" s="55" t="s">
+      <c r="H34" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="I34" s="56" t="s">
+      <c r="I34" s="58" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1913,9 +1949,9 @@
       <c r="F35" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G35" s="55"/>
-      <c r="H35" s="55"/>
-      <c r="I35" s="56"/>
+      <c r="G35" s="57"/>
+      <c r="H35" s="57"/>
+      <c r="I35" s="58"/>
     </row>
     <row r="36" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="E36" s="4" t="s">
@@ -1924,9 +1960,9 @@
       <c r="F36" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G36" s="55"/>
-      <c r="H36" s="55"/>
-      <c r="I36" s="56"/>
+      <c r="G36" s="57"/>
+      <c r="H36" s="57"/>
+      <c r="I36" s="58"/>
     </row>
     <row r="37" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="E37" s="4" t="s">
@@ -1935,9 +1971,9 @@
       <c r="F37" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G37" s="55"/>
-      <c r="H37" s="55"/>
-      <c r="I37" s="56"/>
+      <c r="G37" s="57"/>
+      <c r="H37" s="57"/>
+      <c r="I37" s="58"/>
     </row>
     <row r="40" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A40">
@@ -1955,13 +1991,13 @@
       <c r="F40" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G40" s="55" t="s">
+      <c r="G40" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="H40" s="55" t="s">
+      <c r="H40" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="I40" s="56" t="s">
+      <c r="I40" s="58" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1972,9 +2008,9 @@
       <c r="F41" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G41" s="55"/>
-      <c r="H41" s="55"/>
-      <c r="I41" s="56"/>
+      <c r="G41" s="57"/>
+      <c r="H41" s="57"/>
+      <c r="I41" s="58"/>
     </row>
     <row r="42" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="E42" s="4" t="s">
@@ -1983,9 +2019,9 @@
       <c r="F42" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G42" s="55"/>
-      <c r="H42" s="55"/>
-      <c r="I42" s="56"/>
+      <c r="G42" s="57"/>
+      <c r="H42" s="57"/>
+      <c r="I42" s="58"/>
     </row>
     <row r="43" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="E43" s="4" t="s">
@@ -1994,9 +2030,9 @@
       <c r="F43" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="G43" s="55"/>
-      <c r="H43" s="55"/>
-      <c r="I43" s="56"/>
+      <c r="G43" s="57"/>
+      <c r="H43" s="57"/>
+      <c r="I43" s="58"/>
     </row>
     <row r="46" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A46">
@@ -2014,13 +2050,13 @@
       <c r="F46" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G46" s="55" t="s">
+      <c r="G46" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="H46" s="55" t="s">
+      <c r="H46" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="I46" s="56" t="s">
+      <c r="I46" s="58" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2031,9 +2067,9 @@
       <c r="F47" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G47" s="55"/>
-      <c r="H47" s="55"/>
-      <c r="I47" s="56"/>
+      <c r="G47" s="57"/>
+      <c r="H47" s="57"/>
+      <c r="I47" s="58"/>
     </row>
     <row r="48" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="E48" s="4" t="s">
@@ -2042,9 +2078,9 @@
       <c r="F48" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G48" s="55"/>
-      <c r="H48" s="55"/>
-      <c r="I48" s="56"/>
+      <c r="G48" s="57"/>
+      <c r="H48" s="57"/>
+      <c r="I48" s="58"/>
     </row>
     <row r="49" spans="1:9" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="E49" s="4" t="s">
@@ -2053,9 +2089,9 @@
       <c r="F49" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G49" s="55"/>
-      <c r="H49" s="55"/>
-      <c r="I49" s="56"/>
+      <c r="G49" s="57"/>
+      <c r="H49" s="57"/>
+      <c r="I49" s="58"/>
     </row>
     <row r="52" spans="1:9" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A52">
@@ -2076,13 +2112,13 @@
       <c r="F52" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G52" s="55" t="s">
+      <c r="G52" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="H52" s="55" t="s">
+      <c r="H52" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="I52" s="56" t="s">
+      <c r="I52" s="58" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2093,9 +2129,9 @@
       <c r="F53" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G53" s="55"/>
-      <c r="H53" s="55"/>
-      <c r="I53" s="56"/>
+      <c r="G53" s="57"/>
+      <c r="H53" s="57"/>
+      <c r="I53" s="58"/>
     </row>
     <row r="54" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="E54" s="4" t="s">
@@ -2104,9 +2140,9 @@
       <c r="F54" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G54" s="55"/>
-      <c r="H54" s="55"/>
-      <c r="I54" s="56"/>
+      <c r="G54" s="57"/>
+      <c r="H54" s="57"/>
+      <c r="I54" s="58"/>
     </row>
     <row r="55" spans="1:9" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="E55" s="4" t="s">
@@ -2115,9 +2151,9 @@
       <c r="F55" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="G55" s="55"/>
-      <c r="H55" s="55"/>
-      <c r="I55" s="56"/>
+      <c r="G55" s="57"/>
+      <c r="H55" s="57"/>
+      <c r="I55" s="58"/>
     </row>
     <row r="58" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A58">
@@ -2135,13 +2171,13 @@
       <c r="F58" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G58" s="55" t="s">
+      <c r="G58" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="H58" s="55" t="s">
+      <c r="H58" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="I58" s="56" t="s">
+      <c r="I58" s="58" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2152,9 +2188,9 @@
       <c r="F59" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G59" s="55"/>
-      <c r="H59" s="55"/>
-      <c r="I59" s="56"/>
+      <c r="G59" s="57"/>
+      <c r="H59" s="57"/>
+      <c r="I59" s="58"/>
     </row>
     <row r="60" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="E60" s="4" t="s">
@@ -2163,9 +2199,9 @@
       <c r="F60" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G60" s="55"/>
-      <c r="H60" s="55"/>
-      <c r="I60" s="56"/>
+      <c r="G60" s="57"/>
+      <c r="H60" s="57"/>
+      <c r="I60" s="58"/>
     </row>
     <row r="61" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="E61" s="4" t="s">
@@ -2174,30 +2210,18 @@
       <c r="F61" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G61" s="55"/>
-      <c r="H61" s="55"/>
-      <c r="I61" s="56"/>
+      <c r="G61" s="57"/>
+      <c r="H61" s="57"/>
+      <c r="I61" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="G40:G43"/>
-    <mergeCell ref="H40:H43"/>
-    <mergeCell ref="I40:I43"/>
-    <mergeCell ref="G46:G49"/>
-    <mergeCell ref="H46:H49"/>
-    <mergeCell ref="I46:I49"/>
-    <mergeCell ref="G28:G31"/>
-    <mergeCell ref="H28:H31"/>
-    <mergeCell ref="I28:I31"/>
-    <mergeCell ref="G34:G37"/>
-    <mergeCell ref="H34:H37"/>
-    <mergeCell ref="I34:I37"/>
-    <mergeCell ref="G16:G19"/>
-    <mergeCell ref="H16:H19"/>
-    <mergeCell ref="I16:I19"/>
-    <mergeCell ref="G22:G25"/>
-    <mergeCell ref="H22:H25"/>
-    <mergeCell ref="I22:I25"/>
+    <mergeCell ref="G52:G55"/>
+    <mergeCell ref="H52:H55"/>
+    <mergeCell ref="I52:I55"/>
+    <mergeCell ref="G58:G61"/>
+    <mergeCell ref="H58:H61"/>
+    <mergeCell ref="I58:I61"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G4:G6"/>
     <mergeCell ref="H4:H6"/>
@@ -2205,12 +2229,24 @@
     <mergeCell ref="G9:G13"/>
     <mergeCell ref="H9:H13"/>
     <mergeCell ref="I9:I13"/>
-    <mergeCell ref="G52:G55"/>
-    <mergeCell ref="H52:H55"/>
-    <mergeCell ref="I52:I55"/>
-    <mergeCell ref="G58:G61"/>
-    <mergeCell ref="H58:H61"/>
-    <mergeCell ref="I58:I61"/>
+    <mergeCell ref="G16:G19"/>
+    <mergeCell ref="H16:H19"/>
+    <mergeCell ref="I16:I19"/>
+    <mergeCell ref="G22:G25"/>
+    <mergeCell ref="H22:H25"/>
+    <mergeCell ref="I22:I25"/>
+    <mergeCell ref="G28:G31"/>
+    <mergeCell ref="H28:H31"/>
+    <mergeCell ref="I28:I31"/>
+    <mergeCell ref="G34:G37"/>
+    <mergeCell ref="H34:H37"/>
+    <mergeCell ref="I34:I37"/>
+    <mergeCell ref="G40:G43"/>
+    <mergeCell ref="H40:H43"/>
+    <mergeCell ref="I40:I43"/>
+    <mergeCell ref="G46:G49"/>
+    <mergeCell ref="H46:H49"/>
+    <mergeCell ref="I46:I49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2219,11 +2255,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{048C574D-0BB6-4981-A71F-7914F08050FB}">
-  <dimension ref="A1:N135"/>
+  <dimension ref="A1:N141"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A134" sqref="A134:XFD134"/>
+      <pane ySplit="2" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B141" sqref="B141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2252,10 +2288,10 @@
       <c r="D1" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="80" t="s">
+      <c r="E1" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="80"/>
+      <c r="F1" s="74"/>
       <c r="G1" s="45" t="s">
         <v>5</v>
       </c>
@@ -2314,7 +2350,7 @@
       <c r="G4" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="H4" s="64"/>
+      <c r="H4" s="67"/>
       <c r="I4" s="4"/>
     </row>
     <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2329,7 +2365,7 @@
         <v>70</v>
       </c>
       <c r="G5" s="66"/>
-      <c r="H5" s="64"/>
+      <c r="H5" s="67"/>
       <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:9" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
@@ -2344,7 +2380,7 @@
         <v>72</v>
       </c>
       <c r="G6" s="66"/>
-      <c r="H6" s="64"/>
+      <c r="H6" s="67"/>
       <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:9" s="14" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
@@ -2362,13 +2398,13 @@
       <c r="A8" s="15">
         <v>2</v>
       </c>
-      <c r="B8" s="73" t="s">
+      <c r="B8" s="82" t="s">
         <v>74</v>
       </c>
-      <c r="C8" s="73" t="s">
+      <c r="C8" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="73" t="s">
+      <c r="D8" s="82" t="s">
         <v>77</v>
       </c>
       <c r="E8" s="16" t="s">
@@ -2377,40 +2413,40 @@
       <c r="F8" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="G8" s="76" t="s">
+      <c r="G8" s="80" t="s">
         <v>76</v>
       </c>
-      <c r="H8" s="68"/>
+      <c r="H8" s="78"/>
       <c r="I8" s="17"/>
     </row>
     <row r="9" spans="1:9" ht="46.8" x14ac:dyDescent="0.6">
       <c r="A9" s="18"/>
-      <c r="B9" s="78"/>
-      <c r="C9" s="69"/>
-      <c r="D9" s="78"/>
+      <c r="B9" s="83"/>
+      <c r="C9" s="85"/>
+      <c r="D9" s="83"/>
       <c r="E9" s="16" t="s">
         <v>75</v>
       </c>
       <c r="F9" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="G9" s="77"/>
-      <c r="H9" s="68"/>
+      <c r="G9" s="81"/>
+      <c r="H9" s="78"/>
       <c r="I9" s="17"/>
     </row>
     <row r="10" spans="1:9" ht="31.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A10" s="18"/>
-      <c r="B10" s="79"/>
-      <c r="C10" s="79"/>
-      <c r="D10" s="79"/>
+      <c r="B10" s="84"/>
+      <c r="C10" s="84"/>
+      <c r="D10" s="84"/>
       <c r="E10" s="16" t="s">
         <v>71</v>
       </c>
       <c r="F10" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="G10" s="77"/>
-      <c r="H10" s="68"/>
+      <c r="G10" s="81"/>
+      <c r="H10" s="78"/>
       <c r="I10" s="17"/>
     </row>
     <row r="11" spans="1:9" s="14" customFormat="1" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
@@ -2461,16 +2497,16 @@
       <c r="I13" s="22"/>
     </row>
     <row r="14" spans="1:9" ht="43.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.6">
-      <c r="A14" s="67">
+      <c r="A14" s="79">
         <v>4</v>
       </c>
-      <c r="B14" s="62" t="s">
+      <c r="B14" s="77" t="s">
         <v>83</v>
       </c>
-      <c r="C14" s="73" t="s">
+      <c r="C14" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="62" t="s">
+      <c r="D14" s="77" t="s">
         <v>90</v>
       </c>
       <c r="E14" s="16" t="s">
@@ -2479,70 +2515,70 @@
       <c r="F14" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="G14" s="62" t="s">
+      <c r="G14" s="77" t="s">
         <v>91</v>
       </c>
-      <c r="H14" s="74"/>
+      <c r="H14" s="89"/>
       <c r="I14" s="18"/>
     </row>
     <row r="15" spans="1:9" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A15" s="70"/>
-      <c r="B15" s="63"/>
-      <c r="C15" s="69"/>
-      <c r="D15" s="68"/>
+      <c r="A15" s="86"/>
+      <c r="B15" s="88"/>
+      <c r="C15" s="85"/>
+      <c r="D15" s="78"/>
       <c r="E15" s="16" t="s">
         <v>69</v>
       </c>
       <c r="F15" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="G15" s="68"/>
-      <c r="H15" s="75"/>
+      <c r="G15" s="78"/>
+      <c r="H15" s="90"/>
       <c r="I15" s="18"/>
     </row>
     <row r="16" spans="1:9" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A16" s="70"/>
-      <c r="B16" s="63"/>
-      <c r="C16" s="69"/>
-      <c r="D16" s="68"/>
+      <c r="A16" s="86"/>
+      <c r="B16" s="88"/>
+      <c r="C16" s="85"/>
+      <c r="D16" s="78"/>
       <c r="E16" s="18" t="s">
         <v>86</v>
       </c>
       <c r="F16" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="G16" s="68"/>
-      <c r="H16" s="75"/>
+      <c r="G16" s="78"/>
+      <c r="H16" s="90"/>
       <c r="I16" s="18"/>
     </row>
     <row r="17" spans="1:14" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A17" s="70"/>
-      <c r="B17" s="63"/>
-      <c r="C17" s="69"/>
-      <c r="D17" s="68"/>
+      <c r="A17" s="86"/>
+      <c r="B17" s="88"/>
+      <c r="C17" s="85"/>
+      <c r="D17" s="78"/>
       <c r="E17" s="16" t="s">
         <v>87</v>
       </c>
       <c r="F17" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="G17" s="68"/>
-      <c r="H17" s="75"/>
+      <c r="G17" s="78"/>
+      <c r="H17" s="90"/>
       <c r="I17" s="18"/>
     </row>
     <row r="18" spans="1:14" ht="31.5" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A18" s="71"/>
-      <c r="B18" s="63"/>
-      <c r="C18" s="69"/>
-      <c r="D18" s="68"/>
+      <c r="A18" s="87"/>
+      <c r="B18" s="88"/>
+      <c r="C18" s="85"/>
+      <c r="D18" s="78"/>
       <c r="E18" s="16" t="s">
         <v>94</v>
       </c>
       <c r="F18" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="G18" s="68"/>
-      <c r="H18" s="75"/>
+      <c r="G18" s="78"/>
+      <c r="H18" s="90"/>
       <c r="I18" s="18"/>
     </row>
     <row r="19" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
@@ -2562,16 +2598,16 @@
       <c r="N19" s="14"/>
     </row>
     <row r="20" spans="1:14" ht="52.8" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="67">
+      <c r="A20" s="79">
         <v>5</v>
       </c>
-      <c r="B20" s="62" t="s">
+      <c r="B20" s="77" t="s">
         <v>92</v>
       </c>
-      <c r="C20" s="58" t="s">
+      <c r="C20" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="62" t="s">
+      <c r="D20" s="77" t="s">
         <v>100</v>
       </c>
       <c r="E20" s="25" t="s">
@@ -2580,61 +2616,61 @@
       <c r="F20" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="G20" s="62" t="s">
+      <c r="G20" s="77" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="52.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="70"/>
-      <c r="B21" s="63"/>
-      <c r="C21" s="72"/>
-      <c r="D21" s="68"/>
+      <c r="A21" s="86"/>
+      <c r="B21" s="88"/>
+      <c r="C21" s="70"/>
+      <c r="D21" s="78"/>
       <c r="E21" s="25" t="s">
         <v>69</v>
       </c>
       <c r="F21" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="G21" s="68"/>
+      <c r="G21" s="78"/>
     </row>
     <row r="22" spans="1:14" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A22" s="70"/>
-      <c r="B22" s="63"/>
-      <c r="C22" s="72"/>
-      <c r="D22" s="68"/>
+      <c r="A22" s="86"/>
+      <c r="B22" s="88"/>
+      <c r="C22" s="70"/>
+      <c r="D22" s="78"/>
       <c r="E22" s="17" t="s">
         <v>93</v>
       </c>
       <c r="F22" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="G22" s="68"/>
+      <c r="G22" s="78"/>
     </row>
     <row r="23" spans="1:14" ht="44.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="70"/>
-      <c r="B23" s="63"/>
-      <c r="C23" s="72"/>
-      <c r="D23" s="68"/>
+      <c r="A23" s="86"/>
+      <c r="B23" s="88"/>
+      <c r="C23" s="70"/>
+      <c r="D23" s="78"/>
       <c r="E23" s="25" t="s">
         <v>87</v>
       </c>
       <c r="F23" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="G23" s="68"/>
+      <c r="G23" s="78"/>
     </row>
     <row r="24" spans="1:14" ht="47.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A24" s="70"/>
-      <c r="B24" s="63"/>
-      <c r="C24" s="72"/>
-      <c r="D24" s="68"/>
+      <c r="A24" s="86"/>
+      <c r="B24" s="88"/>
+      <c r="C24" s="70"/>
+      <c r="D24" s="78"/>
       <c r="E24" s="25" t="s">
         <v>95</v>
       </c>
       <c r="F24" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="G24" s="68"/>
+      <c r="G24" s="78"/>
     </row>
     <row r="25" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A25" s="9"/>
@@ -2653,16 +2689,16 @@
       <c r="N25" s="14"/>
     </row>
     <row r="26" spans="1:14" ht="36" customHeight="1" thickTop="1" x14ac:dyDescent="0.6">
-      <c r="A26" s="68">
+      <c r="A26" s="78">
         <v>6</v>
       </c>
-      <c r="B26" s="68" t="s">
+      <c r="B26" s="78" t="s">
         <v>101</v>
       </c>
-      <c r="C26" s="69" t="s">
+      <c r="C26" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="68" t="s">
+      <c r="D26" s="78" t="s">
         <v>137</v>
       </c>
       <c r="E26" s="28" t="s">
@@ -2676,10 +2712,10 @@
       </c>
     </row>
     <row r="27" spans="1:14" ht="31.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="68"/>
-      <c r="B27" s="68"/>
-      <c r="C27" s="64"/>
-      <c r="D27" s="59"/>
+      <c r="A27" s="78"/>
+      <c r="B27" s="78"/>
+      <c r="C27" s="67"/>
+      <c r="D27" s="61"/>
       <c r="E27" s="30" t="s">
         <v>69</v>
       </c>
@@ -2689,10 +2725,10 @@
       <c r="G27" s="66"/>
     </row>
     <row r="28" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A28" s="68"/>
-      <c r="B28" s="68"/>
-      <c r="C28" s="64"/>
-      <c r="D28" s="59"/>
+      <c r="A28" s="78"/>
+      <c r="B28" s="78"/>
+      <c r="C28" s="67"/>
+      <c r="D28" s="61"/>
       <c r="E28" s="29" t="s">
         <v>93</v>
       </c>
@@ -2702,10 +2738,10 @@
       <c r="G28" s="66"/>
     </row>
     <row r="29" spans="1:14" ht="36.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="68"/>
-      <c r="B29" s="68"/>
-      <c r="C29" s="64"/>
-      <c r="D29" s="59"/>
+      <c r="A29" s="78"/>
+      <c r="B29" s="78"/>
+      <c r="C29" s="67"/>
+      <c r="D29" s="61"/>
       <c r="E29" s="30" t="s">
         <v>87</v>
       </c>
@@ -2715,10 +2751,10 @@
       <c r="G29" s="66"/>
     </row>
     <row r="30" spans="1:14" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A30" s="68"/>
-      <c r="B30" s="68"/>
-      <c r="C30" s="64"/>
-      <c r="D30" s="59"/>
+      <c r="A30" s="78"/>
+      <c r="B30" s="78"/>
+      <c r="C30" s="67"/>
+      <c r="D30" s="61"/>
       <c r="E30" s="25" t="s">
         <v>138</v>
       </c>
@@ -2744,16 +2780,16 @@
       <c r="N31" s="14"/>
     </row>
     <row r="32" spans="1:14" ht="39" customHeight="1" thickTop="1" x14ac:dyDescent="0.6">
-      <c r="A32" s="62">
+      <c r="A32" s="77">
         <v>7</v>
       </c>
-      <c r="B32" s="62" t="s">
+      <c r="B32" s="77" t="s">
         <v>102</v>
       </c>
-      <c r="C32" s="67" t="s">
+      <c r="C32" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="D32" s="60" t="s">
+      <c r="D32" s="65" t="s">
         <v>103</v>
       </c>
       <c r="E32" s="16" t="s">
@@ -2767,10 +2803,10 @@
       </c>
     </row>
     <row r="33" spans="1:14" ht="31.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="64"/>
-      <c r="B33" s="64"/>
-      <c r="C33" s="59"/>
-      <c r="D33" s="64"/>
+      <c r="A33" s="67"/>
+      <c r="B33" s="67"/>
+      <c r="C33" s="61"/>
+      <c r="D33" s="67"/>
       <c r="E33" s="25" t="s">
         <v>69</v>
       </c>
@@ -2780,10 +2816,10 @@
       <c r="G33" s="66"/>
     </row>
     <row r="34" spans="1:14" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A34" s="64"/>
-      <c r="B34" s="64"/>
-      <c r="C34" s="59"/>
-      <c r="D34" s="64"/>
+      <c r="A34" s="67"/>
+      <c r="B34" s="67"/>
+      <c r="C34" s="61"/>
+      <c r="D34" s="67"/>
       <c r="E34" s="24" t="s">
         <v>93</v>
       </c>
@@ -2793,10 +2829,10 @@
       <c r="G34" s="66"/>
     </row>
     <row r="35" spans="1:14" ht="25.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="64"/>
-      <c r="B35" s="64"/>
-      <c r="C35" s="59"/>
-      <c r="D35" s="64"/>
+      <c r="A35" s="67"/>
+      <c r="B35" s="67"/>
+      <c r="C35" s="61"/>
+      <c r="D35" s="67"/>
       <c r="E35" s="25" t="s">
         <v>87</v>
       </c>
@@ -2806,10 +2842,10 @@
       <c r="G35" s="66"/>
     </row>
     <row r="36" spans="1:14" ht="31.5" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A36" s="64"/>
-      <c r="B36" s="64"/>
-      <c r="C36" s="59"/>
-      <c r="D36" s="64"/>
+      <c r="A36" s="67"/>
+      <c r="B36" s="67"/>
+      <c r="C36" s="61"/>
+      <c r="D36" s="67"/>
       <c r="E36" s="25" t="s">
         <v>108</v>
       </c>
@@ -2835,16 +2871,16 @@
       <c r="N37" s="14"/>
     </row>
     <row r="38" spans="1:14" ht="4.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.6">
-      <c r="A38" s="62">
+      <c r="A38" s="77">
         <v>8</v>
       </c>
-      <c r="B38" s="62" t="s">
+      <c r="B38" s="77" t="s">
         <v>107</v>
       </c>
-      <c r="C38" s="67" t="s">
+      <c r="C38" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="D38" s="60" t="s">
+      <c r="D38" s="65" t="s">
         <v>103</v>
       </c>
       <c r="E38" s="16"/>
@@ -2854,37 +2890,37 @@
       </c>
     </row>
     <row r="39" spans="1:14" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="64"/>
-      <c r="B39" s="64"/>
-      <c r="C39" s="59"/>
-      <c r="D39" s="64"/>
+      <c r="A39" s="67"/>
+      <c r="B39" s="67"/>
+      <c r="C39" s="61"/>
+      <c r="D39" s="67"/>
       <c r="E39" s="25"/>
       <c r="F39" s="24"/>
       <c r="G39" s="66"/>
     </row>
     <row r="40" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A40" s="64"/>
-      <c r="B40" s="64"/>
-      <c r="C40" s="59"/>
-      <c r="D40" s="64"/>
+      <c r="A40" s="67"/>
+      <c r="B40" s="67"/>
+      <c r="C40" s="61"/>
+      <c r="D40" s="67"/>
       <c r="E40" s="24"/>
       <c r="F40" s="17"/>
       <c r="G40" s="66"/>
     </row>
     <row r="41" spans="1:14" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="64"/>
-      <c r="B41" s="64"/>
-      <c r="C41" s="59"/>
-      <c r="D41" s="64"/>
+      <c r="A41" s="67"/>
+      <c r="B41" s="67"/>
+      <c r="C41" s="61"/>
+      <c r="D41" s="67"/>
       <c r="E41" s="25"/>
       <c r="F41" s="24"/>
       <c r="G41" s="66"/>
     </row>
     <row r="42" spans="1:14" ht="15.9" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A42" s="64"/>
-      <c r="B42" s="64"/>
-      <c r="C42" s="59"/>
-      <c r="D42" s="64"/>
+      <c r="A42" s="67"/>
+      <c r="B42" s="67"/>
+      <c r="C42" s="61"/>
+      <c r="D42" s="67"/>
       <c r="E42" s="25" t="s">
         <v>109</v>
       </c>
@@ -2910,16 +2946,16 @@
       <c r="N43" s="14"/>
     </row>
     <row r="44" spans="1:14" ht="15.9" thickTop="1" x14ac:dyDescent="0.6">
-      <c r="A44" s="62">
+      <c r="A44" s="77">
         <v>9</v>
       </c>
-      <c r="B44" s="62" t="s">
+      <c r="B44" s="77" t="s">
         <v>114</v>
       </c>
-      <c r="C44" s="58" t="s">
+      <c r="C44" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="D44" s="60" t="s">
+      <c r="D44" s="65" t="s">
         <v>103</v>
       </c>
       <c r="E44" s="16"/>
@@ -2929,37 +2965,37 @@
       </c>
     </row>
     <row r="45" spans="1:14" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="64"/>
-      <c r="B45" s="64"/>
-      <c r="C45" s="59"/>
-      <c r="D45" s="64"/>
+      <c r="A45" s="67"/>
+      <c r="B45" s="67"/>
+      <c r="C45" s="61"/>
+      <c r="D45" s="67"/>
       <c r="E45" s="25"/>
       <c r="F45" s="24"/>
       <c r="G45" s="66"/>
     </row>
     <row r="46" spans="1:14" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A46" s="64"/>
-      <c r="B46" s="64"/>
-      <c r="C46" s="59"/>
-      <c r="D46" s="64"/>
+      <c r="A46" s="67"/>
+      <c r="B46" s="67"/>
+      <c r="C46" s="61"/>
+      <c r="D46" s="67"/>
       <c r="E46" s="24"/>
       <c r="F46" s="17"/>
       <c r="G46" s="66"/>
     </row>
     <row r="47" spans="1:14" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="64"/>
-      <c r="B47" s="64"/>
-      <c r="C47" s="59"/>
-      <c r="D47" s="64"/>
+      <c r="A47" s="67"/>
+      <c r="B47" s="67"/>
+      <c r="C47" s="61"/>
+      <c r="D47" s="67"/>
       <c r="E47" s="25"/>
       <c r="F47" s="24"/>
       <c r="G47" s="66"/>
     </row>
     <row r="48" spans="1:14" ht="31.5" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A48" s="64"/>
-      <c r="B48" s="64"/>
-      <c r="C48" s="59"/>
-      <c r="D48" s="64"/>
+      <c r="A48" s="67"/>
+      <c r="B48" s="67"/>
+      <c r="C48" s="61"/>
+      <c r="D48" s="67"/>
       <c r="E48" s="25" t="s">
         <v>112</v>
       </c>
@@ -2985,16 +3021,16 @@
       <c r="N49" s="14"/>
     </row>
     <row r="50" spans="1:14" ht="31.5" thickTop="1" x14ac:dyDescent="0.6">
-      <c r="A50" s="62">
+      <c r="A50" s="77">
         <v>10</v>
       </c>
-      <c r="B50" s="62" t="s">
+      <c r="B50" s="77" t="s">
         <v>115</v>
       </c>
-      <c r="C50" s="58" t="s">
+      <c r="C50" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="D50" s="60" t="s">
+      <c r="D50" s="65" t="s">
         <v>103</v>
       </c>
       <c r="E50" s="16" t="s">
@@ -3008,10 +3044,10 @@
       </c>
     </row>
     <row r="51" spans="1:14" ht="31.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="64"/>
-      <c r="B51" s="64"/>
-      <c r="C51" s="59"/>
-      <c r="D51" s="64"/>
+      <c r="A51" s="67"/>
+      <c r="B51" s="67"/>
+      <c r="C51" s="61"/>
+      <c r="D51" s="67"/>
       <c r="E51" s="25" t="s">
         <v>69</v>
       </c>
@@ -3021,10 +3057,10 @@
       <c r="G51" s="66"/>
     </row>
     <row r="52" spans="1:14" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A52" s="64"/>
-      <c r="B52" s="64"/>
-      <c r="C52" s="59"/>
-      <c r="D52" s="64"/>
+      <c r="A52" s="67"/>
+      <c r="B52" s="67"/>
+      <c r="C52" s="61"/>
+      <c r="D52" s="67"/>
       <c r="E52" s="24" t="s">
         <v>93</v>
       </c>
@@ -3034,10 +3070,10 @@
       <c r="G52" s="66"/>
     </row>
     <row r="53" spans="1:14" ht="31.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A53" s="64"/>
-      <c r="B53" s="64"/>
-      <c r="C53" s="59"/>
-      <c r="D53" s="64"/>
+      <c r="A53" s="67"/>
+      <c r="B53" s="67"/>
+      <c r="C53" s="61"/>
+      <c r="D53" s="67"/>
       <c r="E53" s="25" t="s">
         <v>87</v>
       </c>
@@ -3047,10 +3083,10 @@
       <c r="G53" s="66"/>
     </row>
     <row r="54" spans="1:14" ht="31.5" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A54" s="64"/>
-      <c r="B54" s="64"/>
-      <c r="C54" s="59"/>
-      <c r="D54" s="64"/>
+      <c r="A54" s="67"/>
+      <c r="B54" s="67"/>
+      <c r="C54" s="61"/>
+      <c r="D54" s="67"/>
       <c r="E54" s="25" t="s">
         <v>113</v>
       </c>
@@ -3079,13 +3115,13 @@
       <c r="A56">
         <v>11</v>
       </c>
-      <c r="B56" s="58" t="s">
+      <c r="B56" s="60" t="s">
         <v>116</v>
       </c>
-      <c r="C56" s="58" t="s">
+      <c r="C56" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="D56" s="60" t="s">
+      <c r="D56" s="65" t="s">
         <v>117</v>
       </c>
       <c r="E56" s="16" t="s">
@@ -3094,57 +3130,57 @@
       <c r="F56" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="G56" s="81" t="s">
+      <c r="G56" s="75" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="57" spans="1:14" ht="44.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B57" s="59"/>
-      <c r="C57" s="59"/>
-      <c r="D57" s="59"/>
+      <c r="B57" s="61"/>
+      <c r="C57" s="61"/>
+      <c r="D57" s="61"/>
       <c r="E57" s="25" t="s">
         <v>69</v>
       </c>
       <c r="F57" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="G57" s="82"/>
+      <c r="G57" s="76"/>
     </row>
     <row r="58" spans="1:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B58" s="59"/>
-      <c r="C58" s="59"/>
-      <c r="D58" s="59"/>
+      <c r="B58" s="61"/>
+      <c r="C58" s="61"/>
+      <c r="D58" s="61"/>
       <c r="E58" s="24" t="s">
         <v>93</v>
       </c>
       <c r="F58" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="G58" s="82"/>
+      <c r="G58" s="76"/>
     </row>
     <row r="59" spans="1:14" ht="36.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B59" s="59"/>
-      <c r="C59" s="59"/>
-      <c r="D59" s="59"/>
+      <c r="B59" s="61"/>
+      <c r="C59" s="61"/>
+      <c r="D59" s="61"/>
       <c r="E59" s="25" t="s">
         <v>87</v>
       </c>
       <c r="F59" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="G59" s="82"/>
+      <c r="G59" s="76"/>
     </row>
     <row r="60" spans="1:14" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B60" s="59"/>
-      <c r="C60" s="59"/>
-      <c r="D60" s="59"/>
+      <c r="B60" s="61"/>
+      <c r="C60" s="61"/>
+      <c r="D60" s="61"/>
       <c r="E60" s="25" t="s">
         <v>120</v>
       </c>
       <c r="F60" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="G60" s="82"/>
+      <c r="G60" s="76"/>
     </row>
     <row r="61" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A61" s="9"/>
@@ -3163,16 +3199,16 @@
       <c r="N61" s="14"/>
     </row>
     <row r="62" spans="1:14" ht="31.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.6">
-      <c r="A62" s="58">
+      <c r="A62" s="60">
         <v>12</v>
       </c>
-      <c r="B62" s="58" t="s">
+      <c r="B62" s="60" t="s">
         <v>123</v>
       </c>
-      <c r="C62" s="58" t="s">
+      <c r="C62" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="D62" s="62" t="s">
+      <c r="D62" s="77" t="s">
         <v>124</v>
       </c>
       <c r="E62" s="16" t="s">
@@ -3186,10 +3222,10 @@
       </c>
     </row>
     <row r="63" spans="1:14" ht="31.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A63" s="59"/>
-      <c r="B63" s="59"/>
-      <c r="C63" s="59"/>
-      <c r="D63" s="63"/>
+      <c r="A63" s="61"/>
+      <c r="B63" s="61"/>
+      <c r="C63" s="61"/>
+      <c r="D63" s="88"/>
       <c r="E63" s="25" t="s">
         <v>69</v>
       </c>
@@ -3198,10 +3234,10 @@
       </c>
     </row>
     <row r="64" spans="1:14" ht="31.5" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A64" s="59"/>
-      <c r="B64" s="59"/>
-      <c r="C64" s="59"/>
-      <c r="D64" s="63"/>
+      <c r="A64" s="61"/>
+      <c r="B64" s="61"/>
+      <c r="C64" s="61"/>
+      <c r="D64" s="88"/>
       <c r="E64" s="26" t="s">
         <v>125</v>
       </c>
@@ -3226,16 +3262,16 @@
       <c r="N65" s="14"/>
     </row>
     <row r="66" spans="1:14" ht="31.5" thickTop="1" x14ac:dyDescent="0.6">
-      <c r="A66" s="65">
+      <c r="A66" s="91">
         <v>13</v>
       </c>
-      <c r="B66" s="65" t="s">
+      <c r="B66" s="91" t="s">
         <v>130</v>
       </c>
-      <c r="C66" s="65" t="s">
+      <c r="C66" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="D66" s="62" t="s">
+      <c r="D66" s="77" t="s">
         <v>131</v>
       </c>
       <c r="E66" s="16" t="s">
@@ -3244,48 +3280,48 @@
       <c r="F66" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="G66" s="60" t="s">
+      <c r="G66" s="65" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="67" spans="1:14" ht="31.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A67" s="64"/>
-      <c r="B67" s="64"/>
-      <c r="C67" s="64"/>
-      <c r="D67" s="64"/>
+      <c r="A67" s="67"/>
+      <c r="B67" s="67"/>
+      <c r="C67" s="67"/>
+      <c r="D67" s="67"/>
       <c r="E67" s="25" t="s">
         <v>69</v>
       </c>
       <c r="F67" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="G67" s="61"/>
+      <c r="G67" s="71"/>
     </row>
     <row r="68" spans="1:14" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A68" s="64"/>
-      <c r="B68" s="64"/>
-      <c r="C68" s="64"/>
-      <c r="D68" s="64"/>
+      <c r="A68" s="67"/>
+      <c r="B68" s="67"/>
+      <c r="C68" s="67"/>
+      <c r="D68" s="67"/>
       <c r="E68" s="26" t="s">
         <v>125</v>
       </c>
       <c r="F68" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="G68" s="61"/>
+      <c r="G68" s="71"/>
     </row>
     <row r="69" spans="1:14" ht="15.9" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A69" s="64"/>
-      <c r="B69" s="64"/>
-      <c r="C69" s="64"/>
-      <c r="D69" s="64"/>
+      <c r="A69" s="67"/>
+      <c r="B69" s="67"/>
+      <c r="C69" s="67"/>
+      <c r="D69" s="67"/>
       <c r="E69" s="26" t="s">
         <v>132</v>
       </c>
       <c r="F69" t="s">
         <v>133</v>
       </c>
-      <c r="G69" s="61"/>
+      <c r="G69" s="71"/>
     </row>
     <row r="70" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A70" s="9"/>
@@ -3304,16 +3340,16 @@
       <c r="N70" s="14"/>
     </row>
     <row r="71" spans="1:14" ht="31.5" thickTop="1" x14ac:dyDescent="0.6">
-      <c r="A71" s="58">
+      <c r="A71" s="60">
         <v>14</v>
       </c>
-      <c r="B71" s="62" t="s">
+      <c r="B71" s="77" t="s">
         <v>140</v>
       </c>
-      <c r="C71" s="58" t="s">
+      <c r="C71" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="D71" s="62" t="s">
+      <c r="D71" s="77" t="s">
         <v>124</v>
       </c>
       <c r="E71" s="16" t="s">
@@ -3324,10 +3360,10 @@
       </c>
     </row>
     <row r="72" spans="1:14" ht="31.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A72" s="59"/>
-      <c r="B72" s="63"/>
-      <c r="C72" s="59"/>
-      <c r="D72" s="63"/>
+      <c r="A72" s="61"/>
+      <c r="B72" s="88"/>
+      <c r="C72" s="61"/>
+      <c r="D72" s="88"/>
       <c r="E72" s="25" t="s">
         <v>69</v>
       </c>
@@ -3339,10 +3375,10 @@
       </c>
     </row>
     <row r="73" spans="1:14" ht="38.4" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A73" s="59"/>
-      <c r="B73" s="63"/>
-      <c r="C73" s="59"/>
-      <c r="D73" s="63"/>
+      <c r="A73" s="61"/>
+      <c r="B73" s="88"/>
+      <c r="C73" s="61"/>
+      <c r="D73" s="88"/>
       <c r="E73" s="26" t="s">
         <v>125</v>
       </c>
@@ -3351,10 +3387,10 @@
       </c>
     </row>
     <row r="74" spans="1:14" ht="15.9" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A74" s="64"/>
-      <c r="B74" s="64"/>
-      <c r="C74" s="59"/>
-      <c r="D74" s="64"/>
+      <c r="A74" s="67"/>
+      <c r="B74" s="67"/>
+      <c r="C74" s="61"/>
+      <c r="D74" s="67"/>
       <c r="E74" s="26" t="s">
         <v>135</v>
       </c>
@@ -3418,16 +3454,16 @@
       <c r="N77" s="14"/>
     </row>
     <row r="78" spans="1:14" ht="31.5" thickTop="1" x14ac:dyDescent="0.6">
-      <c r="A78" s="58">
+      <c r="A78" s="60">
         <v>16</v>
       </c>
-      <c r="B78" s="58" t="s">
+      <c r="B78" s="60" t="s">
         <v>151</v>
       </c>
-      <c r="C78" s="58" t="s">
+      <c r="C78" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="D78" s="62" t="s">
+      <c r="D78" s="77" t="s">
         <v>124</v>
       </c>
       <c r="E78" s="16" t="s">
@@ -3436,42 +3472,42 @@
       <c r="F78" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="G78" s="60" t="s">
+      <c r="G78" s="65" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="79" spans="1:14" ht="31.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A79" s="59"/>
-      <c r="B79" s="59"/>
-      <c r="C79" s="59"/>
-      <c r="D79" s="63"/>
+      <c r="A79" s="61"/>
+      <c r="B79" s="61"/>
+      <c r="C79" s="61"/>
+      <c r="D79" s="88"/>
       <c r="E79" s="25" t="s">
         <v>69</v>
       </c>
       <c r="F79" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="G79" s="59"/>
+      <c r="G79" s="61"/>
     </row>
     <row r="80" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A80" s="59"/>
-      <c r="B80" s="59"/>
-      <c r="C80" s="59"/>
-      <c r="D80" s="63"/>
+      <c r="A80" s="61"/>
+      <c r="B80" s="61"/>
+      <c r="C80" s="61"/>
+      <c r="D80" s="88"/>
       <c r="E80" s="32" t="s">
         <v>152</v>
       </c>
       <c r="F80" s="33" t="s">
         <v>153</v>
       </c>
-      <c r="G80" s="59"/>
+      <c r="G80" s="61"/>
     </row>
     <row r="81" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A81" s="59"/>
-      <c r="B81" s="59"/>
-      <c r="C81" s="59"/>
-      <c r="D81" s="64"/>
-      <c r="G81" s="59"/>
+      <c r="A81" s="61"/>
+      <c r="B81" s="61"/>
+      <c r="C81" s="61"/>
+      <c r="D81" s="67"/>
+      <c r="G81" s="61"/>
     </row>
     <row r="82" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A82" s="9"/>
@@ -3490,16 +3526,16 @@
       <c r="N82" s="14"/>
     </row>
     <row r="83" spans="1:14" ht="31.5" thickTop="1" x14ac:dyDescent="0.6">
-      <c r="A83" s="58">
+      <c r="A83" s="60">
         <v>17</v>
       </c>
-      <c r="B83" s="58" t="s">
+      <c r="B83" s="60" t="s">
         <v>148</v>
       </c>
-      <c r="C83" s="58" t="s">
+      <c r="C83" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="D83" s="62" t="s">
+      <c r="D83" s="77" t="s">
         <v>124</v>
       </c>
       <c r="E83" s="16" t="s">
@@ -3508,42 +3544,42 @@
       <c r="F83" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="G83" s="60" t="s">
+      <c r="G83" s="65" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="84" spans="1:14" ht="31.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A84" s="59"/>
-      <c r="B84" s="59"/>
-      <c r="C84" s="59"/>
-      <c r="D84" s="63"/>
+      <c r="A84" s="61"/>
+      <c r="B84" s="61"/>
+      <c r="C84" s="61"/>
+      <c r="D84" s="88"/>
       <c r="E84" s="25" t="s">
         <v>69</v>
       </c>
       <c r="F84" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="G84" s="59"/>
+      <c r="G84" s="61"/>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A85" s="59"/>
-      <c r="B85" s="59"/>
-      <c r="C85" s="59"/>
-      <c r="D85" s="63"/>
+      <c r="A85" s="61"/>
+      <c r="B85" s="61"/>
+      <c r="C85" s="61"/>
+      <c r="D85" s="88"/>
       <c r="E85" s="32" t="s">
         <v>149</v>
       </c>
       <c r="F85" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="G85" s="59"/>
+      <c r="G85" s="61"/>
     </row>
     <row r="86" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A86" s="59"/>
-      <c r="B86" s="59"/>
-      <c r="C86" s="59"/>
-      <c r="D86" s="64"/>
-      <c r="G86" s="59"/>
+      <c r="A86" s="61"/>
+      <c r="B86" s="61"/>
+      <c r="C86" s="61"/>
+      <c r="D86" s="67"/>
+      <c r="G86" s="61"/>
     </row>
     <row r="87" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A87" s="9"/>
@@ -3718,45 +3754,45 @@
       <c r="N95" s="14"/>
     </row>
     <row r="96" spans="1:14" ht="14.7" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A96" s="58">
+      <c r="A96" s="60">
         <v>22</v>
       </c>
-      <c r="B96" s="58" t="s">
+      <c r="B96" s="60" t="s">
         <v>164</v>
       </c>
-      <c r="C96" s="58" t="s">
+      <c r="C96" s="60" t="s">
         <v>165</v>
       </c>
-      <c r="D96" s="87" t="s">
+      <c r="D96" s="68" t="s">
         <v>174</v>
       </c>
-      <c r="E96" s="60" t="s">
+      <c r="E96" s="65" t="s">
         <v>175</v>
       </c>
-      <c r="F96" s="85" t="s">
+      <c r="F96" s="92" t="s">
         <v>176</v>
       </c>
-      <c r="G96" s="83" t="s">
+      <c r="G96" s="62" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A97" s="59"/>
-      <c r="B97" s="59"/>
-      <c r="C97" s="59"/>
-      <c r="D97" s="86"/>
-      <c r="E97" s="59"/>
-      <c r="F97" s="86"/>
-      <c r="G97" s="84"/>
+      <c r="A97" s="61"/>
+      <c r="B97" s="61"/>
+      <c r="C97" s="61"/>
+      <c r="D97" s="69"/>
+      <c r="E97" s="61"/>
+      <c r="F97" s="69"/>
+      <c r="G97" s="63"/>
     </row>
     <row r="98" spans="1:14" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A98" s="59"/>
-      <c r="B98" s="59"/>
-      <c r="C98" s="64"/>
-      <c r="D98" s="64"/>
-      <c r="E98" s="64"/>
-      <c r="F98" s="86"/>
-      <c r="G98" s="84"/>
+      <c r="A98" s="61"/>
+      <c r="B98" s="61"/>
+      <c r="C98" s="67"/>
+      <c r="D98" s="67"/>
+      <c r="E98" s="67"/>
+      <c r="F98" s="69"/>
+      <c r="G98" s="63"/>
     </row>
     <row r="99" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A99" s="9"/>
@@ -3775,38 +3811,38 @@
       <c r="N99" s="14"/>
     </row>
     <row r="100" spans="1:14" ht="40.200000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A100" s="58">
+      <c r="A100" s="60">
         <v>23</v>
       </c>
-      <c r="B100" s="58" t="s">
+      <c r="B100" s="60" t="s">
         <v>178</v>
       </c>
-      <c r="C100" s="58" t="s">
+      <c r="C100" s="60" t="s">
         <v>165</v>
       </c>
-      <c r="D100" s="60" t="s">
+      <c r="D100" s="65" t="s">
         <v>183</v>
       </c>
-      <c r="E100" s="60" t="s">
+      <c r="E100" s="65" t="s">
         <v>180</v>
       </c>
-      <c r="F100" s="83" t="s">
+      <c r="F100" s="62" t="s">
         <v>181</v>
       </c>
-      <c r="G100" s="83" t="s">
+      <c r="G100" s="62" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="101" spans="1:14" ht="36.299999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A101" s="59"/>
-      <c r="B101" s="59"/>
-      <c r="C101" s="59"/>
-      <c r="D101" s="59" t="s">
+      <c r="A101" s="61"/>
+      <c r="B101" s="61"/>
+      <c r="C101" s="61"/>
+      <c r="D101" s="61" t="s">
         <v>179</v>
       </c>
-      <c r="E101" s="59"/>
-      <c r="F101" s="64"/>
-      <c r="G101" s="64"/>
+      <c r="E101" s="61"/>
+      <c r="F101" s="67"/>
+      <c r="G101" s="67"/>
     </row>
     <row r="102" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A102" s="9"/>
@@ -3942,55 +3978,55 @@
       <c r="N108" s="14"/>
     </row>
     <row r="109" spans="1:14" ht="55.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A109" s="58">
+      <c r="A109" s="60">
         <v>27</v>
       </c>
-      <c r="B109" s="58" t="s">
+      <c r="B109" s="60" t="s">
         <v>195</v>
       </c>
-      <c r="C109" s="58" t="s">
+      <c r="C109" s="60" t="s">
         <v>196</v>
       </c>
-      <c r="D109" s="60" t="s">
+      <c r="D109" s="65" t="s">
         <v>197</v>
       </c>
       <c r="E109" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="F109" s="60" t="s">
+      <c r="F109" s="65" t="s">
         <v>200</v>
       </c>
-      <c r="G109" s="60" t="s">
+      <c r="G109" s="65" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="110" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A110" s="72"/>
-      <c r="B110" s="72"/>
-      <c r="C110" s="72"/>
-      <c r="D110" s="61"/>
+      <c r="A110" s="70"/>
+      <c r="B110" s="70"/>
+      <c r="C110" s="70"/>
+      <c r="D110" s="71"/>
       <c r="E110" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="F110" s="61"/>
-      <c r="G110" s="59"/>
+      <c r="F110" s="71"/>
+      <c r="G110" s="61"/>
     </row>
     <row r="111" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A111" s="72"/>
-      <c r="B111" s="72"/>
-      <c r="C111" s="72"/>
-      <c r="D111" s="61"/>
+      <c r="A111" s="70"/>
+      <c r="B111" s="70"/>
+      <c r="C111" s="70"/>
+      <c r="D111" s="71"/>
       <c r="E111" s="53" t="s">
         <v>198</v>
       </c>
-      <c r="F111" s="61"/>
-      <c r="G111" s="59"/>
+      <c r="F111" s="71"/>
+      <c r="G111" s="61"/>
     </row>
     <row r="112" spans="1:14" ht="38.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A112" s="72"/>
-      <c r="B112" s="72"/>
-      <c r="C112" s="72"/>
-      <c r="D112" s="61"/>
+      <c r="A112" s="70"/>
+      <c r="B112" s="70"/>
+      <c r="C112" s="70"/>
+      <c r="D112" s="71"/>
       <c r="E112" s="49" t="s">
         <v>199</v>
       </c>
@@ -4002,10 +4038,10 @@
       </c>
     </row>
     <row r="113" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A113" s="72"/>
-      <c r="B113" s="72"/>
-      <c r="C113" s="72"/>
-      <c r="D113" s="61"/>
+      <c r="A113" s="70"/>
+      <c r="B113" s="70"/>
+      <c r="C113" s="70"/>
+      <c r="D113" s="71"/>
       <c r="E113" s="51" t="s">
         <v>203</v>
       </c>
@@ -4017,10 +4053,10 @@
       </c>
     </row>
     <row r="114" spans="1:14" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A114" s="72"/>
-      <c r="B114" s="72"/>
-      <c r="C114" s="72"/>
-      <c r="D114" s="61"/>
+      <c r="A114" s="70"/>
+      <c r="B114" s="70"/>
+      <c r="C114" s="70"/>
+      <c r="D114" s="71"/>
       <c r="E114" s="48" t="s">
         <v>207</v>
       </c>
@@ -4087,38 +4123,38 @@
       <c r="N117" s="14"/>
     </row>
     <row r="118" spans="1:14" ht="27.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A118" s="58">
+      <c r="A118" s="60">
         <v>29</v>
       </c>
-      <c r="B118" s="58" t="s">
+      <c r="B118" s="60" t="s">
         <v>215</v>
       </c>
-      <c r="C118" s="58" t="s">
+      <c r="C118" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="D118" s="58" t="s">
+      <c r="D118" s="60" t="s">
         <v>210</v>
       </c>
       <c r="E118" s="50" t="s">
         <v>216</v>
       </c>
-      <c r="F118" s="58" t="s">
+      <c r="F118" s="60" t="s">
         <v>218</v>
       </c>
-      <c r="G118" s="88" t="s">
+      <c r="G118" s="72" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="119" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A119" s="59"/>
-      <c r="B119" s="59"/>
-      <c r="C119" s="59"/>
-      <c r="D119" s="59"/>
+      <c r="A119" s="61"/>
+      <c r="B119" s="61"/>
+      <c r="C119" s="61"/>
+      <c r="D119" s="61"/>
       <c r="E119" s="50" t="s">
         <v>217</v>
       </c>
-      <c r="F119" s="59"/>
-      <c r="G119" s="89"/>
+      <c r="F119" s="61"/>
+      <c r="G119" s="73"/>
     </row>
     <row r="120" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A120" s="9"/>
@@ -4137,38 +4173,38 @@
       <c r="N120" s="14"/>
     </row>
     <row r="121" spans="1:14" ht="36" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A121" s="58">
+      <c r="A121" s="60">
         <v>30</v>
       </c>
-      <c r="B121" s="58" t="s">
+      <c r="B121" s="60" t="s">
         <v>220</v>
       </c>
-      <c r="C121" s="58" t="s">
+      <c r="C121" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="D121" s="58" t="s">
+      <c r="D121" s="60" t="s">
         <v>210</v>
       </c>
       <c r="E121" s="50" t="s">
         <v>216</v>
       </c>
-      <c r="F121" s="58" t="s">
+      <c r="F121" s="60" t="s">
         <v>222</v>
       </c>
-      <c r="G121" s="58" t="s">
+      <c r="G121" s="60" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="122" spans="1:14" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A122" s="59"/>
-      <c r="B122" s="59"/>
-      <c r="C122" s="59"/>
-      <c r="D122" s="59"/>
+      <c r="A122" s="61"/>
+      <c r="B122" s="61"/>
+      <c r="C122" s="61"/>
+      <c r="D122" s="61"/>
       <c r="E122" s="50" t="s">
         <v>221</v>
       </c>
-      <c r="F122" s="59"/>
-      <c r="G122" s="59"/>
+      <c r="F122" s="61"/>
+      <c r="G122" s="61"/>
     </row>
     <row r="123" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A123" s="9"/>
@@ -4199,20 +4235,20 @@
       <c r="D124" t="s">
         <v>225</v>
       </c>
-      <c r="E124" s="58" t="s">
+      <c r="E124" s="60" t="s">
         <v>226</v>
       </c>
-      <c r="F124" s="83" t="s">
+      <c r="F124" s="62" t="s">
         <v>227</v>
       </c>
-      <c r="G124" s="83" t="s">
+      <c r="G124" s="62" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="E125" s="59"/>
-      <c r="F125" s="84"/>
-      <c r="G125" s="84"/>
+      <c r="E125" s="61"/>
+      <c r="F125" s="63"/>
+      <c r="G125" s="63"/>
     </row>
     <row r="128" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="129" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
@@ -4271,35 +4307,35 @@
       <c r="N131" s="14"/>
     </row>
     <row r="132" spans="1:14" ht="29.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A132" s="58">
+      <c r="A132" s="60">
         <v>33</v>
       </c>
-      <c r="B132" s="58" t="s">
+      <c r="B132" s="60" t="s">
         <v>233</v>
       </c>
-      <c r="C132" s="58" t="s">
+      <c r="C132" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="D132" s="58" t="s">
+      <c r="D132" s="60" t="s">
         <v>225</v>
       </c>
-      <c r="E132" s="58" t="s">
+      <c r="E132" s="60" t="s">
         <v>234</v>
       </c>
-      <c r="F132" s="83" t="s">
+      <c r="F132" s="62" t="s">
         <v>235</v>
       </c>
-      <c r="G132" s="60" t="s">
+      <c r="G132" s="65" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="133" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A133" s="59"/>
-      <c r="B133" s="59"/>
-      <c r="C133" s="59"/>
-      <c r="D133" s="59"/>
-      <c r="E133" s="59"/>
-      <c r="F133" s="90"/>
+      <c r="A133" s="61"/>
+      <c r="B133" s="61"/>
+      <c r="C133" s="61"/>
+      <c r="D133" s="61"/>
+      <c r="E133" s="61"/>
+      <c r="F133" s="64"/>
       <c r="G133" s="66"/>
     </row>
     <row r="134" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
@@ -4318,104 +4354,92 @@
       <c r="M134" s="14"/>
       <c r="N134" s="14"/>
     </row>
-    <row r="135" spans="1:14" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="135" spans="1:14" ht="24.3" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A135">
+        <v>34</v>
+      </c>
+      <c r="B135" t="s">
+        <v>237</v>
+      </c>
+      <c r="C135" t="s">
+        <v>10</v>
+      </c>
+      <c r="D135" s="55" t="s">
+        <v>225</v>
+      </c>
+      <c r="E135" s="60" t="s">
+        <v>240</v>
+      </c>
+      <c r="F135" s="62" t="s">
+        <v>239</v>
+      </c>
+      <c r="G135" s="65" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="136" spans="1:14" ht="29.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D136" s="55" t="s">
+        <v>238</v>
+      </c>
+      <c r="E136" s="61"/>
+      <c r="F136" s="64"/>
+      <c r="G136" s="61"/>
+    </row>
+    <row r="137" spans="1:14" ht="29.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="E137" s="55" t="s">
+        <v>241</v>
+      </c>
+      <c r="F137" s="55" t="s">
+        <v>242</v>
+      </c>
+      <c r="G137" s="61"/>
+    </row>
+    <row r="138" spans="1:14" ht="21.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="E138" s="55" t="s">
+        <v>243</v>
+      </c>
+      <c r="F138" s="64" t="s">
+        <v>245</v>
+      </c>
+      <c r="G138" s="61"/>
+    </row>
+    <row r="139" spans="1:14" ht="26.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="E139" s="55" t="s">
+        <v>244</v>
+      </c>
+      <c r="F139" s="64"/>
+      <c r="G139" s="61"/>
+    </row>
+    <row r="140" spans="1:14" s="56" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A140" s="9"/>
+      <c r="B140" s="10"/>
+      <c r="C140" s="10"/>
+      <c r="D140" s="10"/>
+      <c r="E140" s="11"/>
+      <c r="F140" s="12"/>
+      <c r="G140" s="10"/>
+      <c r="H140" s="13"/>
+      <c r="I140" s="12"/>
+      <c r="J140" s="14"/>
+      <c r="K140" s="14"/>
+      <c r="L140" s="14"/>
+      <c r="M140" s="14"/>
+      <c r="N140" s="14"/>
+    </row>
+    <row r="141" spans="1:14" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A141">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:N107" xr:uid="{71596E00-9D51-4451-9442-BC138B6C8C5D}">
     <filterColumn colId="4" showButton="0"/>
   </autoFilter>
-  <mergeCells count="116">
-    <mergeCell ref="A132:A133"/>
-    <mergeCell ref="F124:F125"/>
-    <mergeCell ref="G124:G125"/>
-    <mergeCell ref="E124:E125"/>
-    <mergeCell ref="F132:F133"/>
-    <mergeCell ref="G132:G133"/>
-    <mergeCell ref="E132:E133"/>
-    <mergeCell ref="D132:D133"/>
-    <mergeCell ref="B132:B133"/>
-    <mergeCell ref="C132:C133"/>
-    <mergeCell ref="E96:E98"/>
-    <mergeCell ref="D96:D98"/>
-    <mergeCell ref="C96:C98"/>
-    <mergeCell ref="C109:C114"/>
-    <mergeCell ref="B109:B114"/>
-    <mergeCell ref="D109:D114"/>
-    <mergeCell ref="A109:A114"/>
-    <mergeCell ref="G118:G119"/>
-    <mergeCell ref="A118:A119"/>
-    <mergeCell ref="B118:B119"/>
-    <mergeCell ref="C118:C119"/>
-    <mergeCell ref="D118:D119"/>
-    <mergeCell ref="F118:F119"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="G56:G60"/>
-    <mergeCell ref="D56:D60"/>
-    <mergeCell ref="C56:C60"/>
-    <mergeCell ref="G20:G24"/>
-    <mergeCell ref="B38:B42"/>
-    <mergeCell ref="C38:C42"/>
-    <mergeCell ref="D38:D42"/>
-    <mergeCell ref="G38:G42"/>
-    <mergeCell ref="H4:H6"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="B20:B24"/>
-    <mergeCell ref="D20:D24"/>
-    <mergeCell ref="C20:C24"/>
-    <mergeCell ref="C14:C18"/>
-    <mergeCell ref="A20:A24"/>
-    <mergeCell ref="H14:H18"/>
-    <mergeCell ref="G14:G18"/>
-    <mergeCell ref="D14:D18"/>
-    <mergeCell ref="B14:B18"/>
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="C32:C36"/>
-    <mergeCell ref="D32:D36"/>
-    <mergeCell ref="G32:G36"/>
-    <mergeCell ref="A26:A30"/>
-    <mergeCell ref="B26:B30"/>
-    <mergeCell ref="C26:C30"/>
-    <mergeCell ref="D26:D30"/>
-    <mergeCell ref="G26:G30"/>
-    <mergeCell ref="C62:C64"/>
-    <mergeCell ref="B62:B64"/>
-    <mergeCell ref="A62:A64"/>
-    <mergeCell ref="D62:D64"/>
-    <mergeCell ref="A66:A69"/>
-    <mergeCell ref="A38:A42"/>
-    <mergeCell ref="G44:G48"/>
-    <mergeCell ref="A50:A54"/>
-    <mergeCell ref="B50:B54"/>
-    <mergeCell ref="C50:C54"/>
-    <mergeCell ref="D50:D54"/>
-    <mergeCell ref="G50:G54"/>
-    <mergeCell ref="B44:B48"/>
-    <mergeCell ref="A44:A48"/>
-    <mergeCell ref="D44:D48"/>
-    <mergeCell ref="C44:C48"/>
-    <mergeCell ref="B56:B60"/>
-    <mergeCell ref="D78:D81"/>
-    <mergeCell ref="C78:C81"/>
-    <mergeCell ref="B78:B81"/>
-    <mergeCell ref="G78:G81"/>
-    <mergeCell ref="A78:A81"/>
-    <mergeCell ref="A71:A74"/>
-    <mergeCell ref="D71:D74"/>
-    <mergeCell ref="G66:G69"/>
-    <mergeCell ref="D66:D69"/>
-    <mergeCell ref="B66:B69"/>
-    <mergeCell ref="C66:C69"/>
-    <mergeCell ref="C71:C74"/>
-    <mergeCell ref="B71:B74"/>
+  <mergeCells count="120">
+    <mergeCell ref="E135:E136"/>
+    <mergeCell ref="F135:F136"/>
+    <mergeCell ref="F138:F139"/>
+    <mergeCell ref="G135:G139"/>
     <mergeCell ref="A121:A122"/>
     <mergeCell ref="F121:F122"/>
     <mergeCell ref="G121:G122"/>
@@ -4440,6 +4464,98 @@
     <mergeCell ref="A100:A101"/>
     <mergeCell ref="G96:G98"/>
     <mergeCell ref="F96:F98"/>
+    <mergeCell ref="D78:D81"/>
+    <mergeCell ref="C78:C81"/>
+    <mergeCell ref="B78:B81"/>
+    <mergeCell ref="G78:G81"/>
+    <mergeCell ref="A78:A81"/>
+    <mergeCell ref="A71:A74"/>
+    <mergeCell ref="D71:D74"/>
+    <mergeCell ref="G66:G69"/>
+    <mergeCell ref="D66:D69"/>
+    <mergeCell ref="B66:B69"/>
+    <mergeCell ref="C66:C69"/>
+    <mergeCell ref="C71:C74"/>
+    <mergeCell ref="B71:B74"/>
+    <mergeCell ref="C62:C64"/>
+    <mergeCell ref="B62:B64"/>
+    <mergeCell ref="A62:A64"/>
+    <mergeCell ref="D62:D64"/>
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="A38:A42"/>
+    <mergeCell ref="G44:G48"/>
+    <mergeCell ref="A50:A54"/>
+    <mergeCell ref="B50:B54"/>
+    <mergeCell ref="C50:C54"/>
+    <mergeCell ref="D50:D54"/>
+    <mergeCell ref="G50:G54"/>
+    <mergeCell ref="B44:B48"/>
+    <mergeCell ref="A44:A48"/>
+    <mergeCell ref="D44:D48"/>
+    <mergeCell ref="C44:C48"/>
+    <mergeCell ref="B56:B60"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="C32:C36"/>
+    <mergeCell ref="D32:D36"/>
+    <mergeCell ref="G32:G36"/>
+    <mergeCell ref="A26:A30"/>
+    <mergeCell ref="B26:B30"/>
+    <mergeCell ref="C26:C30"/>
+    <mergeCell ref="D26:D30"/>
+    <mergeCell ref="G26:G30"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="B20:B24"/>
+    <mergeCell ref="D20:D24"/>
+    <mergeCell ref="C20:C24"/>
+    <mergeCell ref="C14:C18"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="H14:H18"/>
+    <mergeCell ref="G14:G18"/>
+    <mergeCell ref="D14:D18"/>
+    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="G56:G60"/>
+    <mergeCell ref="D56:D60"/>
+    <mergeCell ref="C56:C60"/>
+    <mergeCell ref="G20:G24"/>
+    <mergeCell ref="B38:B42"/>
+    <mergeCell ref="C38:C42"/>
+    <mergeCell ref="D38:D42"/>
+    <mergeCell ref="G38:G42"/>
+    <mergeCell ref="E96:E98"/>
+    <mergeCell ref="D96:D98"/>
+    <mergeCell ref="C96:C98"/>
+    <mergeCell ref="C109:C114"/>
+    <mergeCell ref="B109:B114"/>
+    <mergeCell ref="D109:D114"/>
+    <mergeCell ref="A109:A114"/>
+    <mergeCell ref="G118:G119"/>
+    <mergeCell ref="A118:A119"/>
+    <mergeCell ref="B118:B119"/>
+    <mergeCell ref="C118:C119"/>
+    <mergeCell ref="D118:D119"/>
+    <mergeCell ref="F118:F119"/>
+    <mergeCell ref="A132:A133"/>
+    <mergeCell ref="F124:F125"/>
+    <mergeCell ref="G124:G125"/>
+    <mergeCell ref="E124:E125"/>
+    <mergeCell ref="F132:F133"/>
+    <mergeCell ref="G132:G133"/>
+    <mergeCell ref="E132:E133"/>
+    <mergeCell ref="D132:D133"/>
+    <mergeCell ref="B132:B133"/>
+    <mergeCell ref="C132:C133"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>